<commit_message>
JNG-884: fix PostgreSQL timestamp data type
</commit_message>
<xml_diff>
--- a/judo-tatami-asm2rdbms/model/RDBMS_Data_Types_Postgres.xlsx
+++ b/judo-tatami-asm2rdbms/model/RDBMS_Data_Types_Postgres.xlsx
@@ -67,7 +67,7 @@
     <t xml:space="preserve">java.time.OffsetDateTime</t>
   </si>
   <si>
-    <t xml:space="preserve">TIMESTAMPZ</t>
+    <t xml:space="preserve">TIMESTAMP WITH TIME ZONE</t>
   </si>
   <si>
     <t xml:space="preserve">java.time.ZonedDateTime</t>
@@ -391,13 +391,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="14.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="14.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>